<commit_message>
Build relationship for preparation stage excluding zoning
</commit_message>
<xml_diff>
--- a/wlb_datastructure.xlsx
+++ b/wlb_datastructure.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/Documents/vscode/lunmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA94B8C-2052-464A-98AF-D754EB17A0D5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4C93E5-9F17-DF47-BF52-A98B0DA67843}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{93BD1B4E-87C1-E746-8052-B34D75FAB036}"/>
+    <workbookView xWindow="-36080" yWindow="720" windowWidth="31800" windowHeight="14260" xr2:uid="{93BD1B4E-87C1-E746-8052-B34D75FAB036}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>);</t>
   </si>
   <si>
-    <t>CREATE TABLE wlb (</t>
-  </si>
-  <si>
     <t>CREATE TABLE wwninfo (</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>MigrationMethod VARCHAR(50),</t>
   </si>
   <si>
-    <t>PowerHAorHACMP VARCHAR(1)</t>
-  </si>
-  <si>
     <t>Hostgroup VARCHAR(50),</t>
   </si>
   <si>
@@ -156,15 +150,9 @@
     <t>HostgroupNum VARCHAR(2)</t>
   </si>
   <si>
-    <t>LUN INT(11),</t>
-  </si>
-  <si>
     <t>LDEV VARCHAR(8),</t>
   </si>
   <si>
-    <t>NumberOfLDEVs INT(11),</t>
-  </si>
-  <si>
     <t>CommandDevice VARCHAR(50),</t>
   </si>
   <si>
@@ -177,7 +165,43 @@
     <t>PackageType VARCHAR(50),</t>
   </si>
   <si>
-    <t>LDEV VARCHAR(50),</t>
+    <t>CREATE TABLE wlb_server (</t>
+  </si>
+  <si>
+    <t>CREATE TABLE wlb_hostgrp_wwn (</t>
+  </si>
+  <si>
+    <t>PowerHAorHACMP VARCHAR(1),</t>
+  </si>
+  <si>
+    <t>Batch VARCHAR(2),</t>
+  </si>
+  <si>
+    <t>Grp VARCHAR(2)</t>
+  </si>
+  <si>
+    <t>};</t>
+  </si>
+  <si>
+    <t>DestLDEV VARCHAR(8),</t>
+  </si>
+  <si>
+    <t>DummyLDEV VARCHAR(8),</t>
+  </si>
+  <si>
+    <t>DummyLDEVName VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>CREATE TABLE virtualization (</t>
+  </si>
+  <si>
+    <t>LUN VARCHAR(4),</t>
+  </si>
+  <si>
+    <t>NumberOfLDEVs VARCHAR(4),</t>
+  </si>
+  <si>
+    <t>ELUNID VARCHAR(4),</t>
   </si>
 </sst>
 </file>
@@ -545,292 +569,342 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C091C11D-5C98-1F46-8493-50857DE491B0}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="4.83203125" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="5.5" customWidth="1"/>
     <col min="6" max="6" width="5.1640625" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.83203125" customWidth="1"/>
-    <col min="9" max="9" width="5" customWidth="1"/>
+    <col min="8" max="8" width="5" customWidth="1"/>
+    <col min="9" max="9" width="5.1640625" customWidth="1"/>
     <col min="10" max="10" width="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.83203125" customWidth="1"/>
+    <col min="12" max="12" width="5" customWidth="1"/>
+    <col min="13" max="13" width="31" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.33203125" customWidth="1"/>
+    <col min="15" max="15" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+        <v>46</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="2"/>
+        <v>30</v>
+      </c>
       <c r="F2" s="2"/>
       <c r="G2" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
       <c r="J2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>32</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
       <c r="D3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+        <v>31</v>
+      </c>
       <c r="G3" t="s">
-        <v>38</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="P3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="D4" t="s">
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="D5" t="s">
+      <c r="J7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="M7" t="s">
+        <v>8</v>
+      </c>
+      <c r="P7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="J8" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
         <v>43</v>
       </c>
-      <c r="J6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="M10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>12</v>
+      </c>
+      <c r="M11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="J7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="M12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J13" t="s">
         <v>45</v>
       </c>
-      <c r="J8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="M13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>29</v>
+      </c>
+      <c r="M15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
         <v>0</v>
       </c>
-      <c r="D9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G13" t="s">
-        <v>49</v>
-      </c>
-      <c r="J13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G14" t="s">
+      <c r="M16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M28" t="s">
         <v>29</v>
       </c>
-      <c r="J14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G15" t="s">
-        <v>30</v>
-      </c>
-      <c r="J15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G16" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J29" t="s">
+    </row>
+    <row r="29" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M29" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>